<commit_message>
update added an end_date in request
</commit_message>
<xml_diff>
--- a/public/templates/iDtr.xlsx
+++ b/public/templates/iDtr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\School Works\boss jis\ojt\iDTR\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B771DF-587B-4418-982F-1398DE053C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57772E96-62C0-417B-867F-CBDC173C2EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{36B0CFA7-E175-4380-91E4-E60204217D3C}"/>
   </bookViews>
@@ -123,6 +123,55 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Civil Service Form No. 48                                                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Empolyee No. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>and arrival Monday</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/Friday </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>as required</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Official hours of arrival </t>
     </r>
     <r>
@@ -132,7 +181,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{      </t>
+      <t xml:space="preserve">      </t>
     </r>
     <r>
       <rPr>
@@ -152,7 +201,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> 10</t>
     </r>
     <r>
       <rPr>
@@ -163,56 +212,7 @@
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">7:20-11:20; 1:00-5:00 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Civil Service Form No. 48                                                                 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Empolyee No. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>and arrival Monday</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">/Friday </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>as required</t>
+      <t xml:space="preserve">:00-12:00; 1:00-7:00 </t>
     </r>
   </si>
 </sst>
@@ -801,14 +801,128 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -854,120 +968,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1283,123 +1283,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82645F5D-FF6E-4704-A5BF-4B0215425F8D}">
-  <dimension ref="B1:H50"/>
+  <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:H44"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:8" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+    </row>
+    <row r="3" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="61"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="43"/>
+      <c r="E10" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="60" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="61"/>
+      <c r="H10" s="46"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -1425,9 +1425,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="7"/>
@@ -1436,443 +1434,124 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6">
-        <v>3</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6">
-        <v>5</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6">
-        <v>7</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6">
-        <v>9</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="9">
+        <f>SUM(G12:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <f>SUM(H12:H13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="62"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="64"/>
     </row>
     <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6">
-        <v>12</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="6">
-        <v>13</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6">
-        <v>14</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="6">
-        <v>15</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6">
+      <c r="B21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="6">
-        <v>17</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="6">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="6">
-        <v>19</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="6">
-        <v>20</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="6">
-        <v>21</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="6">
-        <v>22</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="6">
-        <v>23</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="6">
-        <v>24</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="6">
-        <v>25</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="6">
-        <v>26</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="6">
-        <v>27</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="6">
-        <v>28</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="6">
-        <v>29</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="6">
-        <v>30</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-    </row>
-    <row r="43" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="10">
-        <f>SUM(G12:G41)</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="10">
-        <f>SUM(H12:H42)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="41"/>
-    </row>
-    <row r="45" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="44"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="47"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="48"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="50"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="53"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="24"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="26"/>
-    </row>
-    <row r="50" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="29"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
     <mergeCell ref="B8:H8"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>